<commit_message>
Still can't get this right...
</commit_message>
<xml_diff>
--- a/Lab2/Homework/data.xlsx
+++ b/Lab2/Homework/data.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="114">
+  <si>
+    <t>Subject</t>
+  </si>
   <si>
     <t xml:space="preserve">
 </t>
@@ -746,66 +749,68 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s"/>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -870,62 +875,62 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -990,62 +995,62 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -1110,62 +1115,62 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -1230,62 +1235,62 @@
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142">
@@ -1350,62 +1355,62 @@
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174">
@@ -1470,62 +1475,62 @@
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="206">
@@ -1590,62 +1595,62 @@
     </row>
     <row r="226">
       <c r="A226" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="238">
@@ -1710,62 +1715,62 @@
     </row>
     <row r="258">
       <c r="A258" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270">
@@ -1830,62 +1835,62 @@
     </row>
     <row r="290">
       <c r="A290" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="302">
@@ -1950,62 +1955,62 @@
     </row>
     <row r="322">
       <c r="A322" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="334">
@@ -2070,62 +2075,62 @@
     </row>
     <row r="354">
       <c r="A354" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="366">
@@ -2190,62 +2195,62 @@
     </row>
     <row r="386">
       <c r="A386" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="398">
@@ -2310,62 +2315,62 @@
     </row>
     <row r="418">
       <c r="A418" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="430">
@@ -2430,62 +2435,62 @@
     </row>
     <row r="450">
       <c r="A450" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="462">
@@ -2550,62 +2555,62 @@
     </row>
     <row r="482">
       <c r="A482" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="483">
       <c r="A483" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="484">
       <c r="A484" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="485">
       <c r="A485" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="486">
       <c r="A486" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="487">
       <c r="A487" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="488">
       <c r="A488" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="489">
       <c r="A489" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="490">
       <c r="A490" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="491">
       <c r="A491" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="492">
       <c r="A492" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="493">
       <c r="A493" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="494">
@@ -2670,62 +2675,62 @@
     </row>
     <row r="514">
       <c r="A514" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="515">
       <c r="A515" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="516">
       <c r="A516" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="517">
       <c r="A517" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="518">
       <c r="A518" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="519">
       <c r="A519" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="520">
       <c r="A520" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="521">
       <c r="A521" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="522">
       <c r="A522" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="523">
       <c r="A523" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="524">
       <c r="A524" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="525">
       <c r="A525" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="526">
@@ -2790,62 +2795,62 @@
     </row>
     <row r="546">
       <c r="A546" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="547">
       <c r="A547" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="548">
       <c r="A548" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="549">
       <c r="A549" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="550">
       <c r="A550" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="551">
       <c r="A551" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="552">
       <c r="A552" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="553">
       <c r="A553" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="554">
       <c r="A554" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="555">
       <c r="A555" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="556">
       <c r="A556" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="557">
       <c r="A557" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="558">
@@ -2910,62 +2915,62 @@
     </row>
     <row r="578">
       <c r="A578" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="579">
       <c r="A579" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="580">
       <c r="A580" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="581">
       <c r="A581" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="582">
       <c r="A582" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="583">
       <c r="A583" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="584">
       <c r="A584" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="585">
       <c r="A585" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="586">
       <c r="A586" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="587">
       <c r="A587" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="588">
       <c r="A588" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="589">
       <c r="A589" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="590">
@@ -3030,62 +3035,62 @@
     </row>
     <row r="610">
       <c r="A610" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="611">
       <c r="A611" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="612">
       <c r="A612" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="613">
       <c r="A613" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="614">
       <c r="A614" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="615">
       <c r="A615" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="616">
       <c r="A616" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="617">
       <c r="A617" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="618">
       <c r="A618" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="619">
       <c r="A619" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="620">
       <c r="A620" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="621">
       <c r="A621" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="622">
@@ -3150,62 +3155,62 @@
     </row>
     <row r="642">
       <c r="A642" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="643">
       <c r="A643" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="644">
       <c r="A644" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="645">
       <c r="A645" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="646">
       <c r="A646" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="647">
       <c r="A647" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="648">
       <c r="A648" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="649">
       <c r="A649" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="650">
       <c r="A650" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="651">
       <c r="A651" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="652">
       <c r="A652" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="653">
       <c r="A653" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="654">
@@ -3270,62 +3275,62 @@
     </row>
     <row r="674">
       <c r="A674" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="675">
       <c r="A675" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="676">
       <c r="A676" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="677">
       <c r="A677" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="678">
       <c r="A678" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="679">
       <c r="A679" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="680">
       <c r="A680" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="681">
       <c r="A681" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="682">
       <c r="A682" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="683">
       <c r="A683" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="684">
       <c r="A684" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="685">
       <c r="A685" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="686">
@@ -3390,42 +3395,42 @@
     </row>
     <row r="706">
       <c r="A706" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="707">
       <c r="A707" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="708">
       <c r="A708" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="709">
       <c r="A709" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="710">
       <c r="A710" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="711">
       <c r="A711" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="712">
       <c r="A712" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="713">
       <c r="A713" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="714">
@@ -3490,42 +3495,42 @@
     </row>
     <row r="734">
       <c r="A734" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="735">
       <c r="A735" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="736">
       <c r="A736" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="737">
       <c r="A737" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="738">
       <c r="A738" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="739">
       <c r="A739" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="740">
       <c r="A740" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="741">
       <c r="A741" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="742">

</xml_diff>